<commit_message>
Update deployments & docs
</commit_message>
<xml_diff>
--- a/docs/src/SwipeRight_Load.xlsx
+++ b/docs/src/SwipeRight_Load.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SwipeRight\docs\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2EAEB2-081F-49B4-A033-909634A0FAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC4FDA2-C7C7-4DBA-B25D-48686A95E288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19816B19-863A-43B4-99D7-7E3E4A01A14F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Number of users:</t>
   </si>
@@ -136,6 +136,87 @@
   </si>
   <si>
     <t>Apache Kafka</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Recommendation Service</t>
+  </si>
+  <si>
+    <t>Matching Service</t>
+  </si>
+  <si>
+    <t>Profile Service</t>
+  </si>
+  <si>
+    <t>Chat Service</t>
+  </si>
+  <si>
+    <t>Auth Service</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>Matching</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>FR-03, FR-04, FR-06, FR-08</t>
+  </si>
+  <si>
+    <t>FR-02, FR-05</t>
+  </si>
+  <si>
+    <t>Auth service will be called within most features because some form of authentication is neccessary</t>
+  </si>
+  <si>
+    <t>FR-**</t>
+  </si>
+  <si>
+    <t>Load distribution (avg req/sec)</t>
+  </si>
+  <si>
+    <t>Instances:</t>
+  </si>
+  <si>
+    <t>[cassandra: 1, profile service: 1]</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Avg req/sec % total</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>[GET: api/user]</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Concurrency</t>
+  </si>
+  <si>
+    <t>Cluster Support</t>
+  </si>
+  <si>
+    <t>✔</t>
   </si>
 </sst>
 </file>
@@ -145,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,8 +279,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +320,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -221,12 +343,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -245,13 +369,47 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
+    <cellStyle name="Goed" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Ongeldig" xfId="1" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
@@ -267,16 +425,6 @@
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -291,16 +439,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{440C2A7B-2184-4E27-8664-A1751D3E2D8C}" name="RequestLoadMatrix" displayName="RequestLoadMatrix" ref="A6:E16" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{440C2A7B-2184-4E27-8664-A1751D3E2D8C}" name="RequestLoadMatrix" displayName="RequestLoadMatrix" ref="A6:E16" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A6:E16" xr:uid="{440C2A7B-2184-4E27-8664-A1751D3E2D8C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{27311F5D-F453-40C3-A425-70C0780F9DEB}" name="FR"/>
     <tableColumn id="2" xr3:uid="{601FC6CE-A01A-4114-9D68-A3D24E50FFC8}" name="Once Every (days)"/>
-    <tableColumn id="3" xr3:uid="{59D4163D-7352-4804-AC19-5CC496B7EB0A}" name="Peak (req/seconds)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{59D4163D-7352-4804-AC19-5CC496B7EB0A}" name="Peak (req/seconds)" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{D28D7C3B-46BD-4950-811A-72029CFD2168}" name="Avg  (req/second)">
       <calculatedColumnFormula>($C$3/B7) / 86400</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8214F58-B837-4F72-84D8-EA87A18F3F01}" name="Minimal Base Load (req/sec)" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{C8214F58-B837-4F72-84D8-EA87A18F3F01}" name="Minimal Base Load (req/sec)" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.FLOOR.PRECISE(C7*C4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -312,7 +460,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2830B945-2795-4EF2-A7DB-D9797666145A}" name="Tabel3" displayName="Tabel3" ref="A20:B45" totalsRowCount="1">
   <autoFilter ref="A20:B44" xr:uid="{2830B945-2795-4EF2-A7DB-D9797666145A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E68EA268-2EFB-4CB2-95C5-170254C68B97}" name="Time" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E68EA268-2EFB-4CB2-95C5-170254C68B97}" name="Time" dataDxfId="6" totalsRowDxfId="5"/>
     <tableColumn id="2" xr3:uid="{16064B39-2C5F-450E-AB78-68AAD669CD18}" name="Activity FR-01 - FR09" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Tabel3[Activity FR-01 - FR09])</totalsRowFormula>
     </tableColumn>
@@ -322,12 +470,51 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D92D2343-B8EE-43AE-B8CD-90D5C2247AE3}" name="Tabel1" displayName="Tabel1" ref="A61:C65" totalsRowShown="0">
-  <autoFilter ref="A61:C65" xr:uid="{D92D2343-B8EE-43AE-B8CD-90D5C2247AE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D92D2343-B8EE-43AE-B8CD-90D5C2247AE3}" name="Tabel1" displayName="Tabel1" ref="A74:C78" totalsRowShown="0">
+  <autoFilter ref="A74:C78" xr:uid="{D92D2343-B8EE-43AE-B8CD-90D5C2247AE3}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E44D23E4-7F3E-4DE0-A02F-0376665DB2FC}" name="Profile Service (req/s)"/>
     <tableColumn id="2" xr3:uid="{674255C3-DFAC-4FCF-B9AE-C1DBC53AF1E1}" name="avg response time"/>
     <tableColumn id="3" xr3:uid="{909CF6E0-7B65-4778-A7CE-4954F6D97F77}" name="avg failure rate"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D6E7E852-A0EA-48E1-B5C9-FBC4F97B493C}" name="Tabel5" displayName="Tabel5" ref="A50:B56" totalsRowShown="0">
+  <autoFilter ref="A50:B56" xr:uid="{D6E7E852-A0EA-48E1-B5C9-FBC4F97B493C}"/>
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{BECA73CA-3401-44BA-B518-5A5BE2F62836}" name="Service"/>
+    <tableColumn id="3" xr3:uid="{BF3B414D-A63E-49AB-8BA0-0C47F2075B1B}" name="FR"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A26E1769-E288-40B7-9F50-7726BE7EB126}" name="Tabel6" displayName="Tabel6" ref="D50:F56" totalsRowShown="0">
+  <autoFilter ref="D50:F56" xr:uid="{A26E1769-E288-40B7-9F50-7726BE7EB126}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{046D5670-98DC-46A6-A618-854B66A0C290}" name="Service"/>
+    <tableColumn id="2" xr3:uid="{AD6F40A6-BE89-4BA1-BBE0-E6F640910097}" name="Load distribution (avg req/sec)" dataDxfId="4">
+      <calculatedColumnFormula>SUM(D7)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{D3FECA58-7A54-4FB6-8190-B5BCF6247F02}" name="Avg req/sec % total" dataDxfId="3">
+      <calculatedColumnFormula>(E51/SUM($D$7:$D$15))*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BBD5CA03-6965-4769-94F4-970950BD3461}" name="Tabel8" displayName="Tabel8" ref="A61:C64" totalsRowShown="0">
+  <autoFilter ref="A61:C64" xr:uid="{BBD5CA03-6965-4769-94F4-970950BD3461}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B001E2B5-1893-4B0F-8186-820F42C7496B}" name="Technology"/>
+    <tableColumn id="2" xr3:uid="{402769C2-9352-4638-B65F-72BBE8E0491B}" name="Concurrency" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{0E42D556-418D-417A-A7DC-1D3593EC95E2}" name="Cluster Support" dataDxfId="1" dataCellStyle="Goed"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -630,18 +817,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29133F38-3C05-44AC-AD5A-B7025AEDDB21}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="3" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -688,19 +877,19 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="C7">
         <f>(($C$3/B7)*(MAX(Tabel3[Activity FR-01 - FR09])/100)) / 3600</f>
-        <v>77777.777777777781</v>
+        <v>259259.2592592593</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D15" si="0">($C$3/B7) / 86400</f>
-        <v>32407.407407407409</v>
+        <v>108024.69135802471</v>
       </c>
       <c r="E7">
         <f>((($C$3/B7)*(MIN(Tabel3[Activity FR-01 - FR09])/100)) / 3600) * $C$4</f>
-        <v>8555.5555555555566</v>
+        <v>28518.518518518522</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -708,19 +897,19 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C8">
         <f>(($C$3/B8)*(MAX(Tabel3[Activity FR-01 - FR09])/100)) / 3600</f>
-        <v>3888888.888888889</v>
+        <v>777777.77777777775</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>1620370.3703703703</v>
+        <v>324074.0740740741</v>
       </c>
       <c r="E8">
         <f>((($C$3/B8)*(MIN(Tabel3[Activity FR-01 - FR09])/100)) / 3600) * $C$4</f>
-        <v>427777.77777777781</v>
+        <v>85555.555555555562</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,119 +1269,297 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" t="s">
+        <v>49</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51">
+        <f>ROUND(SUM(D7),1)</f>
+        <v>108024.7</v>
+      </c>
+      <c r="F51" s="12">
+        <f>ROUND((E51/SUM($D$7:$D$15))*100,1)</f>
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52">
+        <f>ROUND(SUM(D8,D11),1)</f>
+        <v>356481.5</v>
+      </c>
+      <c r="F52" s="12">
+        <f t="shared" ref="F52:F55" si="1">ROUND((E52/SUM($D$7:$D$15))*100,1)</f>
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53">
+        <f>ROUND(SUM(D9,D10,D12,D14),1)</f>
+        <v>64859.199999999997</v>
+      </c>
+      <c r="F53" s="12">
+        <f t="shared" si="1"/>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54">
+        <f>ROUND(SUM(D7),1)</f>
+        <v>108024.7</v>
+      </c>
+      <c r="F54" s="12">
+        <f t="shared" si="1"/>
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55">
+        <f>ROUND(SUM(D7:D15),1)</f>
+        <v>707606.1</v>
+      </c>
+      <c r="F55" s="12">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="12"/>
+    </row>
+    <row r="59" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B62" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B63" s="17"/>
+      <c r="C63" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
+      <c r="B64" s="17"/>
+      <c r="C64" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C69" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B71" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B72" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B74" t="s">
         <v>26</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>10</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B75" s="4">
         <v>1.7819999999999999E-2</v>
       </c>
-      <c r="C62" s="8">
+      <c r="C75" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>100</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="8">
+      <c r="C76" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>1000</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C77" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>10000</v>
       </c>
-      <c r="B65" s="11">
+      <c r="B78" s="11">
         <v>2.7431000000000001</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C78" s="10">
         <v>0.47</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B21:B44">
-    <cfRule type="top10" dxfId="5" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C59" r:id="rId1" xr:uid="{7717F489-D50B-4988-816E-96F7FEB3811C}"/>
+    <hyperlink ref="C69" r:id="rId1" xr:uid="{7717F489-D50B-4988-816E-96F7FEB3811C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
-  <tableParts count="3">
+  <tableParts count="6">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1342,26 +1709,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31D935B-2FBD-4384-8976-CF2AE76F3C6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E2D53C-897F-48A6-B9F7-96BB27579285}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="50489db6-5088-4038-82a1-52fa82448584"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1385,9 +1741,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E2D53C-897F-48A6-B9F7-96BB27579285}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31D935B-2FBD-4384-8976-CF2AE76F3C6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50489db6-5088-4038-82a1-52fa82448584"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>